<commit_message>
Excel_ReadWrite_Utility has been Implemented Sucessfully
</commit_message>
<xml_diff>
--- a/bin/com/SpiceTG/TestDataFiles/Testdata_1.xlsx
+++ b/bin/com/SpiceTG/TestDataFiles/Testdata_1.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginScreen" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Test_Case_Name</t>
   </si>
@@ -33,6 +33,9 @@
     <t>Actual_Results</t>
   </si>
   <si>
+    <t>Result</t>
+  </si>
+  <si>
     <t>Valid Username and Valid Password Login Test</t>
   </si>
   <si>
@@ -45,38 +48,78 @@
     <t>Login Success</t>
   </si>
   <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>Empty Username and Empty Password Login Test</t>
   </si>
   <si>
+    <t>leo_1</t>
+  </si>
+  <si>
     <t>Login Fail</t>
   </si>
   <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>Valid Username and Empty Password Login Test</t>
   </si>
   <si>
+    <t>leo_12</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
     <t>Valid Username and Invalid Password Login Test</t>
   </si>
   <si>
+    <t>leo_1234</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
     <t>Invalid Username and Valid Password Login Test</t>
   </si>
   <si>
+    <t>leo_123456</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
     <t>Invalid Username and Empty Login Test</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>fails</t>
+    <t>leo_123457</t>
+  </si>
+  <si>
+    <t>Test6</t>
+  </si>
+  <si>
+    <t>leo_123458</t>
+  </si>
+  <si>
+    <t>Test7</t>
+  </si>
+  <si>
+    <t>TestResult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,15 +133,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -150,32 +184,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -471,173 +495,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="2" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.34765625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" t="s" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="6"/>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="G5"/>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" t="s">
-        <v>17</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="A2" r:id="rId6"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B3" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Multiple user name and password from excel file
</commit_message>
<xml_diff>
--- a/bin/com/SpiceTG/TestDataFiles/Testdata_1.xlsx
+++ b/bin/com/SpiceTG/TestDataFiles/Testdata_1.xlsx
@@ -42,9 +42,6 @@
     <t>prasadn@leotechnosoft.net</t>
   </si>
   <si>
-    <t>leo_12345</t>
-  </si>
-  <si>
     <t>Login Success</t>
   </si>
   <si>
@@ -112,13 +109,15 @@
   </si>
   <si>
     <t>TestResult</t>
+  </si>
+  <si>
+    <t>leo_123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -498,19 +497,19 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
-    <col min="2" max="6" style="1" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.34765625" collapsed="true"/>
-    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="6" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -530,11 +529,11 @@
         <v>5</v>
       </c>
       <c r="G1" s="5"/>
-      <c r="H1" t="s" s="6">
-        <v>31</v>
+      <c r="H1" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -542,164 +541,164 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G2"/>
       <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G3"/>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4"/>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5"/>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get UserName and Password from Excel file and if any Alert come then handel that alert
</commit_message>
<xml_diff>
--- a/bin/com/SpiceTG/TestDataFiles/Testdata_1.xlsx
+++ b/bin/com/SpiceTG/TestDataFiles/Testdata_1.xlsx
@@ -42,6 +42,9 @@
     <t>prasadn@leotechnosoft.net</t>
   </si>
   <si>
+    <t>leo_12345</t>
+  </si>
+  <si>
     <t>Login Success</t>
   </si>
   <si>
@@ -109,15 +112,13 @@
   </si>
   <si>
     <t>TestResult</t>
-  </si>
-  <si>
-    <t>leo_123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -497,19 +498,19 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="6" width="9.140625" style="1" collapsed="1"/>
-    <col min="7" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="2" max="6" style="1" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.34765625" collapsed="true"/>
+    <col min="9" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -529,11 +530,11 @@
         <v>5</v>
       </c>
       <c r="G1" s="5"/>
-      <c r="H1" s="6" t="s">
-        <v>30</v>
+      <c r="H1" t="s" s="6">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -541,164 +542,164 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2"/>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3"/>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4"/>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5"/>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8"/>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>